<commit_message>
Update product data with a new category to improve matching accuracy
Replaced "Product Data.xlsx" in /data and /attached_assets to include the missing "Door Type" column.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 0646a5b4-ba54-4146-8119-cc31c948a5ea
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/873c23c0-c18f-4e09-9f8d-38c5cb319996/5d0f7db4-507b-4418-a677-f0a0b4fd794b.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/Product Data_05_13_2025.xlsx
+++ b/attached_assets/Product Data_05_13_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bathcraft-my.sharepoint.com/personal/olep00903843_maax_com/Documents/PythonScripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_BCFEBD4F73F15EB6C55EF89F1835901893D73E67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD788D93-1E4D-4C33-9ADB-4CF5C955C1FB}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_BCFEBD4F73F15EB6C55EF89F1835901893D73E67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5664ADD-B78D-44FB-A7E4-01628B76D406}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-2640" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2565" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shower Bases" sheetId="1" r:id="rId1"/>
@@ -31,16 +31,29 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Screens!$A$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Shower Doors'!$A$1:$O$219</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Showers!$A$1:$I$151</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Tub Doors'!$A$1:$J$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Tub Doors'!$A$1:$K$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Tub Showers'!$A$1:$H$105</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Walls!$A$1:$L$34</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8423" uniqueCount="1974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8468" uniqueCount="1975">
   <si>
     <t>Unique ID</t>
   </si>
@@ -5962,6 +5975,9 @@
   </si>
   <si>
     <t>Reveal Sleek 71 Return Panel for 34 in.</t>
+  </si>
+  <si>
+    <t>Door  Type</t>
   </si>
 </sst>
 </file>
@@ -6063,6 +6079,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16073,12 +16093,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:N156"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="205.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -36826,10 +36849,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36840,12 +36863,13 @@
     <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -36865,111 +36889,123 @@
         <v>1181</v>
       </c>
       <c r="G1" t="s">
+        <v>1974</v>
+      </c>
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>1110</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1782</v>
+        <v>1855</v>
       </c>
       <c r="B2" t="s">
-        <v>1783</v>
+        <v>1856</v>
       </c>
       <c r="D2" t="s">
-        <v>778</v>
+        <v>553</v>
       </c>
       <c r="E2" t="s">
-        <v>895</v>
+        <v>1371</v>
       </c>
       <c r="F2" t="s">
-        <v>1784</v>
+        <v>924</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>1293</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>1347</v>
+        <v>309</v>
       </c>
       <c r="J2" t="s">
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1857</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1785</v>
+        <v>1811</v>
       </c>
       <c r="B3" t="s">
-        <v>1786</v>
+        <v>1812</v>
       </c>
       <c r="D3" t="s">
-        <v>778</v>
+        <v>1303</v>
       </c>
       <c r="E3" t="s">
-        <v>895</v>
+        <v>1055</v>
       </c>
       <c r="F3" t="s">
-        <v>895</v>
+        <v>878</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>1245</v>
+        <v>309</v>
       </c>
       <c r="J3" t="s">
-        <v>1211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1214</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1787</v>
+        <v>1821</v>
       </c>
       <c r="B4" t="s">
-        <v>1788</v>
+        <v>1822</v>
       </c>
       <c r="D4" t="s">
-        <v>521</v>
+        <v>1055</v>
       </c>
       <c r="E4" t="s">
         <v>895</v>
       </c>
       <c r="F4" t="s">
-        <v>895</v>
+        <v>878</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>1498</v>
+        <v>309</v>
       </c>
       <c r="J4" t="s">
-        <v>1499</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1214</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1789</v>
+        <v>1871</v>
       </c>
       <c r="B5" t="s">
-        <v>1790</v>
+        <v>1822</v>
       </c>
       <c r="D5" t="s">
         <v>1055</v>
@@ -36981,111 +37017,123 @@
         <v>878</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H5" t="s">
-        <v>312</v>
+        <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>1251</v>
+        <v>309</v>
       </c>
       <c r="J5" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1214</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1791</v>
+        <v>1797</v>
       </c>
       <c r="B6" t="s">
-        <v>1792</v>
+        <v>1798</v>
       </c>
       <c r="D6" t="s">
-        <v>558</v>
+        <v>1055</v>
       </c>
       <c r="E6" t="s">
-        <v>1371</v>
+        <v>895</v>
       </c>
       <c r="F6" t="s">
-        <v>778</v>
+        <v>878</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>1362</v>
+        <v>309</v>
       </c>
       <c r="J6" t="s">
-        <v>1363</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1214</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1793</v>
+        <v>1804</v>
       </c>
       <c r="B7" t="s">
-        <v>1794</v>
+        <v>1805</v>
       </c>
       <c r="D7" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E7" t="s">
         <v>1055</v>
-      </c>
-      <c r="E7" t="s">
-        <v>895</v>
       </c>
       <c r="F7" t="s">
         <v>878</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
         <v>309</v>
       </c>
-      <c r="I7" t="s">
-        <v>1466</v>
-      </c>
       <c r="J7" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1278</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1795</v>
+        <v>1836</v>
       </c>
       <c r="B8" t="s">
-        <v>1796</v>
+        <v>1837</v>
       </c>
       <c r="D8" t="s">
-        <v>1303</v>
+        <v>1055</v>
       </c>
       <c r="E8" t="s">
-        <v>1055</v>
+        <v>895</v>
       </c>
       <c r="F8" t="s">
         <v>878</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H8" t="s">
-        <v>312</v>
+        <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>1298</v>
+        <v>309</v>
       </c>
       <c r="J8" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1278</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1797</v>
+        <v>1845</v>
       </c>
       <c r="B9" t="s">
-        <v>1798</v>
+        <v>1488</v>
       </c>
       <c r="D9" t="s">
         <v>1055</v>
@@ -37097,401 +37145,443 @@
         <v>878</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" t="s">
         <v>309</v>
       </c>
-      <c r="I9" t="s">
-        <v>1214</v>
-      </c>
       <c r="J9" t="s">
+        <v>1278</v>
+      </c>
+      <c r="K9" t="s">
         <v>1215</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1799</v>
+        <v>1846</v>
       </c>
       <c r="B10" t="s">
-        <v>1800</v>
+        <v>1847</v>
       </c>
       <c r="D10" t="s">
-        <v>1352</v>
+        <v>924</v>
       </c>
       <c r="E10" t="s">
-        <v>935</v>
+        <v>878</v>
       </c>
       <c r="F10" t="s">
+        <v>878</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1293</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>309</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1294</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1851</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1852</v>
+      </c>
+      <c r="D11" t="s">
+        <v>878</v>
+      </c>
+      <c r="E11" t="s">
+        <v>502</v>
+      </c>
+      <c r="F11" t="s">
+        <v>878</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1293</v>
+      </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" t="s">
+        <v>309</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1294</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1809</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1810</v>
+      </c>
+      <c r="E12" t="s">
+        <v>956</v>
+      </c>
+      <c r="F12" t="s">
         <v>778</v>
       </c>
-      <c r="G10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="G12" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" t="s">
         <v>21</v>
       </c>
-      <c r="I10" t="s">
-        <v>1231</v>
-      </c>
-      <c r="J10" t="s">
-        <v>1232</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="J12" t="s">
+        <v>1362</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1792</v>
+      </c>
+      <c r="D13" t="s">
+        <v>558</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1371</v>
+      </c>
+      <c r="F13" t="s">
+        <v>778</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1362</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1807</v>
+      </c>
+      <c r="D14" t="s">
+        <v>778</v>
+      </c>
+      <c r="E14" t="s">
+        <v>895</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1055</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1210</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1787</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1788</v>
+      </c>
+      <c r="D15" t="s">
+        <v>521</v>
+      </c>
+      <c r="E15" t="s">
+        <v>895</v>
+      </c>
+      <c r="F15" t="s">
+        <v>895</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" t="s">
+        <v>1498</v>
+      </c>
+      <c r="K15" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1848</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1849</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E16" t="s">
+        <v>553</v>
+      </c>
+      <c r="F16" t="s">
+        <v>956</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1850</v>
+      </c>
+      <c r="K16" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1873</v>
+      </c>
+      <c r="D17" t="s">
+        <v>778</v>
+      </c>
+      <c r="E17" t="s">
+        <v>895</v>
+      </c>
+      <c r="F17" t="s">
+        <v>956</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1850</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1853</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1854</v>
+      </c>
+      <c r="D18" t="s">
+        <v>778</v>
+      </c>
+      <c r="E18" t="s">
+        <v>895</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1037</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1850</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>1801</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B19" t="s">
         <v>1802</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D19" t="s">
         <v>778</v>
-      </c>
-      <c r="E11" t="s">
-        <v>895</v>
-      </c>
-      <c r="F11" t="s">
-        <v>956</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" t="s">
-        <v>1803</v>
-      </c>
-      <c r="J11" t="s">
-        <v>1192</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>1804</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1805</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1303</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1055</v>
-      </c>
-      <c r="F12" t="s">
-        <v>878</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" t="s">
-        <v>309</v>
-      </c>
-      <c r="I12" t="s">
-        <v>1278</v>
-      </c>
-      <c r="J12" t="s">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>1806</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1807</v>
-      </c>
-      <c r="D13" t="s">
-        <v>778</v>
-      </c>
-      <c r="E13" t="s">
-        <v>895</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1055</v>
-      </c>
-      <c r="G13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" t="s">
-        <v>1210</v>
-      </c>
-      <c r="J13" t="s">
-        <v>1211</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>1808</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1809</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1810</v>
-      </c>
-      <c r="E14" t="s">
-        <v>956</v>
-      </c>
-      <c r="F14" t="s">
-        <v>778</v>
-      </c>
-      <c r="G14" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" t="s">
-        <v>1362</v>
-      </c>
-      <c r="J14" t="s">
-        <v>1363</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>1811</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1812</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1303</v>
-      </c>
-      <c r="E15" t="s">
-        <v>1055</v>
-      </c>
-      <c r="F15" t="s">
-        <v>878</v>
-      </c>
-      <c r="G15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" t="s">
-        <v>309</v>
-      </c>
-      <c r="I15" t="s">
-        <v>1214</v>
-      </c>
-      <c r="J15" t="s">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>1813</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1814</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1718</v>
-      </c>
-      <c r="E16" t="s">
-        <v>502</v>
-      </c>
-      <c r="F16" t="s">
-        <v>878</v>
-      </c>
-      <c r="G16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" t="s">
-        <v>309</v>
-      </c>
-      <c r="I16" t="s">
-        <v>1710</v>
-      </c>
-      <c r="J16" t="s">
-        <v>1711</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>1815</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1816</v>
-      </c>
-      <c r="D17" t="s">
-        <v>553</v>
-      </c>
-      <c r="E17" t="s">
-        <v>1371</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1686</v>
-      </c>
-      <c r="G17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" t="s">
-        <v>309</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1475</v>
-      </c>
-      <c r="J17" t="s">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>1817</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1818</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1303</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1055</v>
-      </c>
-      <c r="F18" t="s">
-        <v>878</v>
-      </c>
-      <c r="G18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" t="s">
-        <v>312</v>
-      </c>
-      <c r="I18" t="s">
-        <v>1251</v>
-      </c>
-      <c r="J18" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>1819</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1820</v>
-      </c>
-      <c r="D19" t="s">
-        <v>521</v>
       </c>
       <c r="E19" t="s">
         <v>895</v>
       </c>
       <c r="F19" t="s">
-        <v>895</v>
+        <v>956</v>
       </c>
       <c r="G19" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H19" t="s">
-        <v>347</v>
+        <v>20</v>
       </c>
       <c r="I19" t="s">
-        <v>1542</v>
+        <v>21</v>
       </c>
       <c r="J19" t="s">
-        <v>1543</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1803</v>
+      </c>
+      <c r="K19" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1821</v>
+        <v>1785</v>
       </c>
       <c r="B20" t="s">
-        <v>1822</v>
+        <v>1786</v>
       </c>
       <c r="D20" t="s">
-        <v>1055</v>
+        <v>778</v>
       </c>
       <c r="E20" t="s">
         <v>895</v>
       </c>
       <c r="F20" t="s">
-        <v>878</v>
+        <v>895</v>
       </c>
       <c r="G20" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H20" t="s">
-        <v>309</v>
+        <v>20</v>
       </c>
       <c r="I20" t="s">
-        <v>1214</v>
+        <v>21</v>
       </c>
       <c r="J20" t="s">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1245</v>
+      </c>
+      <c r="K20" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>1823</v>
+        <v>1817</v>
       </c>
       <c r="B21" t="s">
-        <v>1824</v>
+        <v>1818</v>
       </c>
       <c r="D21" t="s">
-        <v>1357</v>
+        <v>1303</v>
       </c>
       <c r="E21" t="s">
         <v>1055</v>
       </c>
       <c r="F21" t="s">
-        <v>778</v>
+        <v>878</v>
       </c>
       <c r="G21" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>1231</v>
+        <v>312</v>
       </c>
       <c r="J21" t="s">
-        <v>1232</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1251</v>
+      </c>
+      <c r="K21" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>1825</v>
+        <v>1789</v>
       </c>
       <c r="B22" t="s">
-        <v>1826</v>
+        <v>1790</v>
       </c>
       <c r="D22" t="s">
         <v>1055</v>
       </c>
       <c r="E22" t="s">
-        <v>1371</v>
+        <v>895</v>
       </c>
       <c r="F22" t="s">
         <v>878</v>
       </c>
       <c r="G22" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I22" t="s">
-        <v>1270</v>
+        <v>312</v>
       </c>
       <c r="J22" t="s">
-        <v>1271</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1251</v>
+      </c>
+      <c r="K22" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1827</v>
+        <v>1834</v>
       </c>
       <c r="B23" t="s">
-        <v>1828</v>
+        <v>1835</v>
       </c>
       <c r="D23" t="s">
         <v>1055</v>
@@ -37503,53 +37593,59 @@
         <v>878</v>
       </c>
       <c r="G23" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" t="s">
         <v>312</v>
       </c>
-      <c r="I23" t="s">
-        <v>1298</v>
-      </c>
       <c r="J23" t="s">
+        <v>1251</v>
+      </c>
+      <c r="K23" t="s">
         <v>1242</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>1829</v>
+        <v>1795</v>
       </c>
       <c r="B24" t="s">
-        <v>1830</v>
+        <v>1796</v>
       </c>
       <c r="D24" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E24" t="s">
         <v>1055</v>
-      </c>
-      <c r="E24" t="s">
-        <v>895</v>
       </c>
       <c r="F24" t="s">
         <v>878</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H24" t="s">
-        <v>309</v>
+        <v>20</v>
       </c>
       <c r="I24" t="s">
-        <v>1831</v>
+        <v>312</v>
       </c>
       <c r="J24" t="s">
+        <v>1298</v>
+      </c>
+      <c r="K24" t="s">
         <v>1242</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1832</v>
+        <v>1869</v>
       </c>
       <c r="B25" t="s">
-        <v>1833</v>
+        <v>1870</v>
       </c>
       <c r="D25" t="s">
         <v>1055</v>
@@ -37561,24 +37657,27 @@
         <v>878</v>
       </c>
       <c r="G25" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H25" t="s">
-        <v>309</v>
+        <v>20</v>
       </c>
       <c r="I25" t="s">
-        <v>1382</v>
+        <v>312</v>
       </c>
       <c r="J25" t="s">
+        <v>1298</v>
+      </c>
+      <c r="K25" t="s">
         <v>1242</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1834</v>
+        <v>1827</v>
       </c>
       <c r="B26" t="s">
-        <v>1835</v>
+        <v>1828</v>
       </c>
       <c r="D26" t="s">
         <v>1055</v>
@@ -37590,285 +37689,315 @@
         <v>878</v>
       </c>
       <c r="G26" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" t="s">
         <v>312</v>
       </c>
-      <c r="I26" t="s">
-        <v>1251</v>
-      </c>
       <c r="J26" t="s">
+        <v>1298</v>
+      </c>
+      <c r="K26" t="s">
         <v>1242</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>1836</v>
+        <v>1859</v>
       </c>
       <c r="B27" t="s">
-        <v>1837</v>
+        <v>1860</v>
       </c>
       <c r="D27" t="s">
-        <v>1055</v>
+        <v>521</v>
       </c>
       <c r="E27" t="s">
         <v>895</v>
       </c>
       <c r="F27" t="s">
-        <v>878</v>
+        <v>924</v>
       </c>
       <c r="G27" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H27" t="s">
-        <v>309</v>
+        <v>20</v>
       </c>
       <c r="I27" t="s">
-        <v>1278</v>
+        <v>21</v>
       </c>
       <c r="J27" t="s">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1425</v>
+      </c>
+      <c r="K27" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1838</v>
+        <v>1865</v>
       </c>
       <c r="B28" t="s">
-        <v>1839</v>
+        <v>1866</v>
       </c>
       <c r="D28" t="s">
+        <v>553</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1371</v>
+      </c>
+      <c r="F28" t="s">
         <v>1055</v>
       </c>
-      <c r="E28" t="s">
-        <v>895</v>
-      </c>
-      <c r="F28" t="s">
-        <v>878</v>
-      </c>
       <c r="G28" t="s">
-        <v>20</v>
+        <v>1293</v>
       </c>
       <c r="H28" t="s">
-        <v>309</v>
+        <v>20</v>
       </c>
       <c r="I28" t="s">
-        <v>1241</v>
+        <v>21</v>
       </c>
       <c r="J28" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1857</v>
+      </c>
+      <c r="K28" t="s">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1840</v>
+        <v>1829</v>
       </c>
       <c r="B29" t="s">
-        <v>1820</v>
+        <v>1830</v>
       </c>
       <c r="D29" t="s">
-        <v>521</v>
+        <v>1055</v>
       </c>
       <c r="E29" t="s">
         <v>895</v>
       </c>
       <c r="F29" t="s">
+        <v>878</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1293</v>
+      </c>
+      <c r="H29" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" t="s">
+        <v>309</v>
+      </c>
+      <c r="J29" t="s">
+        <v>1831</v>
+      </c>
+      <c r="K29" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1833</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E30" t="s">
         <v>895</v>
       </c>
-      <c r="G29" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" t="s">
-        <v>347</v>
-      </c>
-      <c r="I29" t="s">
-        <v>1542</v>
-      </c>
-      <c r="J29" t="s">
-        <v>1543</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>1841</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1842</v>
-      </c>
-      <c r="D30" t="s">
-        <v>558</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
+        <v>878</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1293</v>
+      </c>
+      <c r="H30" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" t="s">
+        <v>309</v>
+      </c>
+      <c r="J30" t="s">
+        <v>1382</v>
+      </c>
+      <c r="K30" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1814</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1718</v>
+      </c>
+      <c r="E31" t="s">
+        <v>502</v>
+      </c>
+      <c r="F31" t="s">
+        <v>878</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1293</v>
+      </c>
+      <c r="H31" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" t="s">
+        <v>309</v>
+      </c>
+      <c r="J31" t="s">
+        <v>1710</v>
+      </c>
+      <c r="K31" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1816</v>
+      </c>
+      <c r="D32" t="s">
+        <v>553</v>
+      </c>
+      <c r="E32" t="s">
         <v>1371</v>
       </c>
-      <c r="F30" t="s">
-        <v>778</v>
-      </c>
-      <c r="G30" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I30" t="s">
-        <v>1231</v>
-      </c>
-      <c r="J30" t="s">
-        <v>1232</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>1843</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1844</v>
-      </c>
-      <c r="D31" t="s">
-        <v>778</v>
-      </c>
-      <c r="E31" t="s">
-        <v>895</v>
-      </c>
-      <c r="F31" t="s">
-        <v>1784</v>
-      </c>
-      <c r="G31" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" t="s">
-        <v>21</v>
-      </c>
-      <c r="I31" t="s">
-        <v>1347</v>
-      </c>
-      <c r="J31" t="s">
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>1845</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1488</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="F32" t="s">
+        <v>1686</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1293</v>
+      </c>
+      <c r="H32" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" t="s">
+        <v>309</v>
+      </c>
+      <c r="J32" t="s">
+        <v>1475</v>
+      </c>
+      <c r="K32" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1826</v>
+      </c>
+      <c r="D33" t="s">
         <v>1055</v>
       </c>
-      <c r="E32" t="s">
-        <v>895</v>
-      </c>
-      <c r="F32" t="s">
-        <v>878</v>
-      </c>
-      <c r="G32" t="s">
-        <v>20</v>
-      </c>
-      <c r="H32" t="s">
-        <v>309</v>
-      </c>
-      <c r="I32" t="s">
-        <v>1278</v>
-      </c>
-      <c r="J32" t="s">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>1846</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1847</v>
-      </c>
-      <c r="D33" t="s">
-        <v>924</v>
-      </c>
       <c r="E33" t="s">
-        <v>878</v>
+        <v>1371</v>
       </c>
       <c r="F33" t="s">
         <v>878</v>
       </c>
       <c r="G33" t="s">
-        <v>20</v>
+        <v>1293</v>
       </c>
       <c r="H33" t="s">
-        <v>309</v>
+        <v>20</v>
       </c>
       <c r="I33" t="s">
-        <v>1294</v>
+        <v>21</v>
       </c>
       <c r="J33" t="s">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1270</v>
+      </c>
+      <c r="K33" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1848</v>
+        <v>1843</v>
       </c>
       <c r="B34" t="s">
-        <v>1849</v>
+        <v>1844</v>
       </c>
       <c r="D34" t="s">
-        <v>1303</v>
+        <v>778</v>
       </c>
       <c r="E34" t="s">
-        <v>553</v>
+        <v>895</v>
       </c>
       <c r="F34" t="s">
-        <v>956</v>
+        <v>1784</v>
       </c>
       <c r="G34" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H34" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" t="s">
         <v>21</v>
       </c>
-      <c r="I34" t="s">
-        <v>1850</v>
-      </c>
       <c r="J34" t="s">
-        <v>1192</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1347</v>
+      </c>
+      <c r="K34" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1851</v>
+        <v>1782</v>
       </c>
       <c r="B35" t="s">
-        <v>1852</v>
+        <v>1783</v>
       </c>
       <c r="D35" t="s">
-        <v>878</v>
+        <v>778</v>
       </c>
       <c r="E35" t="s">
-        <v>502</v>
+        <v>895</v>
       </c>
       <c r="F35" t="s">
-        <v>878</v>
+        <v>1784</v>
       </c>
       <c r="G35" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H35" t="s">
-        <v>309</v>
+        <v>20</v>
       </c>
       <c r="I35" t="s">
-        <v>1294</v>
+        <v>21</v>
       </c>
       <c r="J35" t="s">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1347</v>
+      </c>
+      <c r="K35" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>1853</v>
+        <v>1861</v>
       </c>
       <c r="B36" t="s">
-        <v>1854</v>
+        <v>1862</v>
       </c>
       <c r="D36" t="s">
         <v>778</v>
@@ -37877,284 +38006,318 @@
         <v>895</v>
       </c>
       <c r="F36" t="s">
-        <v>1037</v>
+        <v>1784</v>
       </c>
       <c r="G36" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H36" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" t="s">
         <v>21</v>
       </c>
-      <c r="I36" t="s">
-        <v>1850</v>
-      </c>
       <c r="J36" t="s">
-        <v>1192</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1274</v>
+      </c>
+      <c r="K36" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>1855</v>
+        <v>1867</v>
       </c>
       <c r="B37" t="s">
-        <v>1856</v>
+        <v>1868</v>
       </c>
       <c r="D37" t="s">
-        <v>553</v>
+        <v>778</v>
       </c>
       <c r="E37" t="s">
-        <v>1371</v>
+        <v>895</v>
       </c>
       <c r="F37" t="s">
-        <v>924</v>
+        <v>1784</v>
       </c>
       <c r="G37" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H37" t="s">
-        <v>309</v>
+        <v>20</v>
       </c>
       <c r="I37" t="s">
-        <v>1857</v>
+        <v>21</v>
       </c>
       <c r="J37" t="s">
-        <v>1858</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1274</v>
+      </c>
+      <c r="K37" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>1859</v>
+        <v>1793</v>
       </c>
       <c r="B38" t="s">
-        <v>1860</v>
+        <v>1794</v>
       </c>
       <c r="D38" t="s">
-        <v>521</v>
+        <v>1055</v>
       </c>
       <c r="E38" t="s">
         <v>895</v>
       </c>
       <c r="F38" t="s">
-        <v>924</v>
+        <v>878</v>
       </c>
       <c r="G38" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I38" t="s">
-        <v>1425</v>
+        <v>309</v>
       </c>
       <c r="J38" t="s">
-        <v>1426</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1466</v>
+      </c>
+      <c r="K38" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>1861</v>
+        <v>1838</v>
       </c>
       <c r="B39" t="s">
-        <v>1862</v>
+        <v>1839</v>
       </c>
       <c r="D39" t="s">
-        <v>778</v>
+        <v>1055</v>
       </c>
       <c r="E39" t="s">
         <v>895</v>
       </c>
       <c r="F39" t="s">
-        <v>1784</v>
+        <v>878</v>
       </c>
       <c r="G39" t="s">
-        <v>20</v>
+        <v>1190</v>
       </c>
       <c r="H39" t="s">
+        <v>20</v>
+      </c>
+      <c r="I39" t="s">
+        <v>309</v>
+      </c>
+      <c r="J39" t="s">
+        <v>1241</v>
+      </c>
+      <c r="K39" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1800</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E40" t="s">
+        <v>935</v>
+      </c>
+      <c r="F40" t="s">
+        <v>778</v>
+      </c>
+      <c r="G40" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H40" t="s">
+        <v>20</v>
+      </c>
+      <c r="I40" t="s">
         <v>21</v>
       </c>
-      <c r="I39" t="s">
-        <v>1274</v>
-      </c>
-      <c r="J39" t="s">
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="J40" t="s">
+        <v>1231</v>
+      </c>
+      <c r="K40" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1824</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1357</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F41" t="s">
+        <v>778</v>
+      </c>
+      <c r="G41" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H41" t="s">
+        <v>20</v>
+      </c>
+      <c r="I41" t="s">
+        <v>21</v>
+      </c>
+      <c r="J41" t="s">
+        <v>1231</v>
+      </c>
+      <c r="K41" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>1841</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1842</v>
+      </c>
+      <c r="D42" t="s">
+        <v>558</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1371</v>
+      </c>
+      <c r="F42" t="s">
+        <v>778</v>
+      </c>
+      <c r="G42" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H42" t="s">
+        <v>20</v>
+      </c>
+      <c r="I42" t="s">
+        <v>21</v>
+      </c>
+      <c r="J42" t="s">
+        <v>1231</v>
+      </c>
+      <c r="K42" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>1863</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" t="s">
         <v>1864</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D43" t="s">
         <v>778</v>
-      </c>
-      <c r="E40" t="s">
-        <v>895</v>
-      </c>
-      <c r="F40" t="s">
-        <v>1672</v>
-      </c>
-      <c r="G40" t="s">
-        <v>20</v>
-      </c>
-      <c r="H40" t="s">
-        <v>21</v>
-      </c>
-      <c r="I40" t="s">
-        <v>1322</v>
-      </c>
-      <c r="J40" t="s">
-        <v>1323</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>1865</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1866</v>
-      </c>
-      <c r="D41" t="s">
-        <v>553</v>
-      </c>
-      <c r="E41" t="s">
-        <v>1371</v>
-      </c>
-      <c r="F41" t="s">
-        <v>1055</v>
-      </c>
-      <c r="G41" t="s">
-        <v>20</v>
-      </c>
-      <c r="H41" t="s">
-        <v>21</v>
-      </c>
-      <c r="I41" t="s">
-        <v>1857</v>
-      </c>
-      <c r="J41" t="s">
-        <v>1858</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>1867</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1868</v>
-      </c>
-      <c r="D42" t="s">
-        <v>778</v>
-      </c>
-      <c r="E42" t="s">
-        <v>895</v>
-      </c>
-      <c r="F42" t="s">
-        <v>1784</v>
-      </c>
-      <c r="G42" t="s">
-        <v>20</v>
-      </c>
-      <c r="H42" t="s">
-        <v>21</v>
-      </c>
-      <c r="I42" t="s">
-        <v>1274</v>
-      </c>
-      <c r="J42" t="s">
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>1869</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1870</v>
-      </c>
-      <c r="D43" t="s">
-        <v>1055</v>
       </c>
       <c r="E43" t="s">
         <v>895</v>
       </c>
       <c r="F43" t="s">
-        <v>878</v>
+        <v>1672</v>
       </c>
       <c r="G43" t="s">
-        <v>20</v>
+        <v>1293</v>
       </c>
       <c r="H43" t="s">
-        <v>312</v>
+        <v>20</v>
       </c>
       <c r="I43" t="s">
-        <v>1298</v>
+        <v>21</v>
       </c>
       <c r="J43" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1322</v>
+      </c>
+      <c r="K43" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1871</v>
+        <v>1819</v>
       </c>
       <c r="B44" t="s">
-        <v>1822</v>
+        <v>1820</v>
       </c>
       <c r="D44" t="s">
-        <v>1055</v>
+        <v>521</v>
       </c>
       <c r="E44" t="s">
         <v>895</v>
       </c>
       <c r="F44" t="s">
-        <v>878</v>
+        <v>895</v>
       </c>
       <c r="G44" t="s">
-        <v>20</v>
+        <v>1293</v>
       </c>
       <c r="H44" t="s">
-        <v>309</v>
+        <v>20</v>
       </c>
       <c r="I44" t="s">
-        <v>1214</v>
+        <v>347</v>
       </c>
       <c r="J44" t="s">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1542</v>
+      </c>
+      <c r="K44" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1872</v>
+        <v>1840</v>
       </c>
       <c r="B45" t="s">
-        <v>1873</v>
+        <v>1820</v>
       </c>
       <c r="D45" t="s">
-        <v>778</v>
+        <v>521</v>
       </c>
       <c r="E45" t="s">
         <v>895</v>
       </c>
       <c r="F45" t="s">
-        <v>956</v>
+        <v>895</v>
       </c>
       <c r="G45" t="s">
-        <v>20</v>
+        <v>1293</v>
       </c>
       <c r="H45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I45" t="s">
-        <v>1850</v>
+        <v>347</v>
       </c>
       <c r="J45" t="s">
-        <v>1192</v>
+        <v>1542</v>
+      </c>
+      <c r="K45" t="s">
+        <v>1543</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J45" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
+  <autoFilter ref="A1:K45" xr:uid="{00000000-0009-0000-0000-000007000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K45">
+      <sortCondition ref="B1:B45"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>